<commit_message>
Add AssetsLoder/Test card loading.
</commit_message>
<xml_diff>
--- a/Product/SettingSource/role_card.xlsx
+++ b/Product/SettingSource/role_card.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="35">
   <si>
     <t>id</t>
   </si>
@@ -127,6 +127,30 @@
   </si>
   <si>
     <t>德行</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>logic_res</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>string</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>独特逻辑</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>tex</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>caocao</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>贴图</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -473,15 +497,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F16"/>
+  <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -500,8 +524,14 @@
       <c r="F1" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G1" t="s">
+        <v>29</v>
+      </c>
+      <c r="H1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -520,8 +550,14 @@
       <c r="F2" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G2" t="s">
+        <v>30</v>
+      </c>
+      <c r="H2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>23</v>
       </c>
@@ -540,8 +576,14 @@
       <c r="F3" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G3" t="s">
+        <v>31</v>
+      </c>
+      <c r="H3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A4">
         <v>1</v>
       </c>
@@ -561,7 +603,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A5">
         <v>2</v>
       </c>
@@ -572,7 +614,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A6">
         <v>3</v>
       </c>
@@ -583,7 +625,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A7">
         <v>4</v>
       </c>
@@ -594,7 +636,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A8">
         <v>5</v>
       </c>
@@ -605,7 +647,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A9">
         <v>6</v>
       </c>
@@ -616,7 +658,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A10">
         <v>7</v>
       </c>
@@ -635,8 +677,11 @@
       <c r="F10">
         <v>5</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="H10" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A11">
         <v>8</v>
       </c>
@@ -647,7 +692,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A12">
         <v>9</v>
       </c>
@@ -658,7 +703,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A13">
         <v>10</v>
       </c>
@@ -669,7 +714,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A14">
         <v>11</v>
       </c>
@@ -680,7 +725,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A15">
         <v>12</v>
       </c>
@@ -691,7 +736,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A16">
         <v>13</v>
       </c>

</xml_diff>

<commit_message>
Add EventSys/AssetsLoader Test/Card UI/Model/xls design.
</commit_message>
<xml_diff>
--- a/Product/SettingSource/role_card.xlsx
+++ b/Product/SettingSource/role_card.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="38">
   <si>
     <t>id</t>
   </si>
@@ -151,6 +151,18 @@
   </si>
   <si>
     <t>贴图</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>model_res</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>string</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>model逻辑</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -497,15 +509,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H16"/>
+  <dimension ref="A1:I16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+      <selection activeCell="I1" sqref="I1:I1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -530,8 +542,11 @@
       <c r="H1" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="I1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -556,8 +571,11 @@
       <c r="H2" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="I2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>23</v>
       </c>
@@ -582,8 +600,11 @@
       <c r="H3" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="I3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A4">
         <v>1</v>
       </c>
@@ -603,7 +624,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A5">
         <v>2</v>
       </c>
@@ -614,7 +635,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A6">
         <v>3</v>
       </c>
@@ -625,7 +646,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A7">
         <v>4</v>
       </c>
@@ -636,7 +657,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A8">
         <v>5</v>
       </c>
@@ -647,7 +668,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A9">
         <v>6</v>
       </c>
@@ -658,7 +679,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A10">
         <v>7</v>
       </c>
@@ -681,7 +702,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A11">
         <v>8</v>
       </c>
@@ -692,7 +713,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A12">
         <v>9</v>
       </c>
@@ -703,7 +724,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A13">
         <v>10</v>
       </c>
@@ -714,7 +735,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A14">
         <v>11</v>
       </c>
@@ -725,7 +746,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A15">
         <v>12</v>
       </c>
@@ -736,7 +757,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A16">
         <v>13</v>
       </c>

</xml_diff>